<commit_message>
Add logos to the advertising media data export
Update the Excel export to include the logo for each advertising media channel.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 68475520-624d-41ed-80f7-0899dcb22821
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 1bbaa446-73d2-4058-b157-dcf80a6b4a7a
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/1ae4e1d9-d8f9-4127-aae8-efcc50d459ff/68475520-624d-41ed-80f7-0899dcb22821/aLuANUi
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/public/tippingpoint_광고매체_데이터.xlsx
+++ b/public/tippingpoint_광고매체_데이터.xlsx
@@ -11,11 +11,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
   <si>
     <t>카테고리</t>
   </si>
   <si>
+    <t>로고</t>
+  </si>
+  <si>
     <t>채널명</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
   </si>
   <si>
     <t>시니어 팬덤 채널</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>서진대학</t>
@@ -262,9 +268,6 @@
   <si>
     <t xml:space="preserve">트롯매거진은 대한민국을 대표하는 국내 최초 트로트 전문 미디어로 트로트 가수·트로트 방송·트로트 이슈를 가장 신속하고 깊이 있게 전달하는 대한민국 No.1 트로트 뉴스 플랫폼입니다.
 우리는 국내 최대 규모의 트로트 전문 콘텐츠를 생산·유통하며, 트로트 산업 발전과 대중문화 확산에 앞장서고 있습니다.</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>블로그</t>
@@ -381,6 +384,440 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>17999</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>89999</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="476250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>17999</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>89999</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="476250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>17999</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>89999</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="476250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>17999</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="476250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>17999</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="476250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>17999</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="476250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>17999</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="476250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>17999</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="476250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>17999</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="476250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>17999</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="476250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>17999</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="476250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -705,7 +1142,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -715,16 +1152,17 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="60" customWidth="1"/>
-    <col min="8" max="9" width="45" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="60" customWidth="1"/>
+    <col min="9" max="10" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="30" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -752,303 +1190,336 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" ht="40" customHeight="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" ht="60" customHeight="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" ht="60" customHeight="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>17</v>
+      <c r="C3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="3" ht="40" customHeight="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="4" t="s">
+    <row r="4" ht="60" customHeight="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>25</v>
+      <c r="H4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="4" ht="40" customHeight="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>31</v>
+    <row r="5" ht="60" customHeight="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="5" ht="40" customHeight="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="4" t="s">
+    <row r="6" ht="60" customHeight="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>39</v>
+      <c r="G6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="6" ht="40" customHeight="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>46</v>
+    <row r="7" ht="60" customHeight="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="7" ht="40" customHeight="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="4" t="s">
+    <row r="8" ht="60" customHeight="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" ht="60" customHeight="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" ht="60" customHeight="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" ht="60" customHeight="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>55</v>
+      <c r="D11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="8" ht="40" customHeight="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" ht="40" customHeight="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" ht="40" customHeight="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" ht="40" customHeight="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" ht="40" customHeight="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" ht="60" customHeight="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>86</v>
@@ -1070,10 +1541,14 @@
       </c>
       <c r="I12" s="4" t="s">
         <v>92</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>